<commit_message>
Déplacement de toutes les variables et des formules dans un fichier XLSX.
</commit_message>
<xml_diff>
--- a/Projet.xlsx
+++ b/Projet.xlsx
@@ -107,15 +107,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
+    <numFmt numFmtId="166" formatCode="##0.0E+0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -138,6 +140,21 @@
       <name val="Ubuntu Mono"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -208,7 +225,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,7 +238,4204 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Puissance utilisée du train lors du trajet</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P_mecanique</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$6:$A$639</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="634"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>274</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>287</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>291</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>296</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>302</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>319</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>322</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>323</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>343</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>346</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>348</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>349</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>351</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>363</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>364</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>367</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>369</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>371</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>372</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>377</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>382</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>383</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>387</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>389</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>393</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>396</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>397</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>401</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>406</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>408</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>409</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>411</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>427</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>437</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>442</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>443</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>446</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="451">
+                  <c:v>451</c:v>
+                </c:pt>
+                <c:pt idx="452">
+                  <c:v>452</c:v>
+                </c:pt>
+                <c:pt idx="453">
+                  <c:v>453</c:v>
+                </c:pt>
+                <c:pt idx="454">
+                  <c:v>454</c:v>
+                </c:pt>
+                <c:pt idx="455">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="456">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="457">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="458">
+                  <c:v>458</c:v>
+                </c:pt>
+                <c:pt idx="459">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="460">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="461">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="462">
+                  <c:v>462</c:v>
+                </c:pt>
+                <c:pt idx="463">
+                  <c:v>463</c:v>
+                </c:pt>
+                <c:pt idx="464">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="465">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="466">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="467">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="468">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="469">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="470">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="471">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="472">
+                  <c:v>472</c:v>
+                </c:pt>
+                <c:pt idx="473">
+                  <c:v>473</c:v>
+                </c:pt>
+                <c:pt idx="474">
+                  <c:v>474</c:v>
+                </c:pt>
+                <c:pt idx="475">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="476">
+                  <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="477">
+                  <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="478">
+                  <c:v>478</c:v>
+                </c:pt>
+                <c:pt idx="479">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="480">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="481">
+                  <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="482">
+                  <c:v>482</c:v>
+                </c:pt>
+                <c:pt idx="483">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="484">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="485">
+                  <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="486">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="487">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="488">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="489">
+                  <c:v>489</c:v>
+                </c:pt>
+                <c:pt idx="490">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="491">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="492">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="493">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="494">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="495">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="496">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="497">
+                  <c:v>497</c:v>
+                </c:pt>
+                <c:pt idx="498">
+                  <c:v>498</c:v>
+                </c:pt>
+                <c:pt idx="499">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="500">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="501">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="502">
+                  <c:v>502</c:v>
+                </c:pt>
+                <c:pt idx="503">
+                  <c:v>503</c:v>
+                </c:pt>
+                <c:pt idx="504">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="505">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="506">
+                  <c:v>506</c:v>
+                </c:pt>
+                <c:pt idx="507">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="508">
+                  <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="509">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="510">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="511">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="512">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="513">
+                  <c:v>513</c:v>
+                </c:pt>
+                <c:pt idx="514">
+                  <c:v>514</c:v>
+                </c:pt>
+                <c:pt idx="515">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="516">
+                  <c:v>516</c:v>
+                </c:pt>
+                <c:pt idx="517">
+                  <c:v>517</c:v>
+                </c:pt>
+                <c:pt idx="518">
+                  <c:v>518</c:v>
+                </c:pt>
+                <c:pt idx="519">
+                  <c:v>519</c:v>
+                </c:pt>
+                <c:pt idx="520">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="521">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="522">
+                  <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="523">
+                  <c:v>523</c:v>
+                </c:pt>
+                <c:pt idx="524">
+                  <c:v>524</c:v>
+                </c:pt>
+                <c:pt idx="525">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="526">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="527">
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="528">
+                  <c:v>528</c:v>
+                </c:pt>
+                <c:pt idx="529">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="530">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="531">
+                  <c:v>531</c:v>
+                </c:pt>
+                <c:pt idx="532">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="533">
+                  <c:v>533</c:v>
+                </c:pt>
+                <c:pt idx="534">
+                  <c:v>534</c:v>
+                </c:pt>
+                <c:pt idx="535">
+                  <c:v>535</c:v>
+                </c:pt>
+                <c:pt idx="536">
+                  <c:v>536</c:v>
+                </c:pt>
+                <c:pt idx="537">
+                  <c:v>537</c:v>
+                </c:pt>
+                <c:pt idx="538">
+                  <c:v>538</c:v>
+                </c:pt>
+                <c:pt idx="539">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="540">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="541">
+                  <c:v>541</c:v>
+                </c:pt>
+                <c:pt idx="542">
+                  <c:v>542</c:v>
+                </c:pt>
+                <c:pt idx="543">
+                  <c:v>543</c:v>
+                </c:pt>
+                <c:pt idx="544">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="545">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="546">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="547">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="548">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="549">
+                  <c:v>549</c:v>
+                </c:pt>
+                <c:pt idx="550">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="551">
+                  <c:v>551</c:v>
+                </c:pt>
+                <c:pt idx="552">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="553">
+                  <c:v>553</c:v>
+                </c:pt>
+                <c:pt idx="554">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="555">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="556">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="557">
+                  <c:v>557</c:v>
+                </c:pt>
+                <c:pt idx="558">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="559">
+                  <c:v>559</c:v>
+                </c:pt>
+                <c:pt idx="560">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="561">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="562">
+                  <c:v>562</c:v>
+                </c:pt>
+                <c:pt idx="563">
+                  <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="564">
+                  <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="565">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="566">
+                  <c:v>566</c:v>
+                </c:pt>
+                <c:pt idx="567">
+                  <c:v>567</c:v>
+                </c:pt>
+                <c:pt idx="568">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="569">
+                  <c:v>569</c:v>
+                </c:pt>
+                <c:pt idx="570">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="571">
+                  <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="572">
+                  <c:v>572</c:v>
+                </c:pt>
+                <c:pt idx="573">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="574">
+                  <c:v>574</c:v>
+                </c:pt>
+                <c:pt idx="575">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="576">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="577">
+                  <c:v>577</c:v>
+                </c:pt>
+                <c:pt idx="578">
+                  <c:v>578</c:v>
+                </c:pt>
+                <c:pt idx="579">
+                  <c:v>579</c:v>
+                </c:pt>
+                <c:pt idx="580">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="581">
+                  <c:v>581</c:v>
+                </c:pt>
+                <c:pt idx="582">
+                  <c:v>582</c:v>
+                </c:pt>
+                <c:pt idx="583">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="584">
+                  <c:v>584</c:v>
+                </c:pt>
+                <c:pt idx="585">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="586">
+                  <c:v>586</c:v>
+                </c:pt>
+                <c:pt idx="587">
+                  <c:v>587</c:v>
+                </c:pt>
+                <c:pt idx="588">
+                  <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="589">
+                  <c:v>589</c:v>
+                </c:pt>
+                <c:pt idx="590">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="591">
+                  <c:v>591</c:v>
+                </c:pt>
+                <c:pt idx="592">
+                  <c:v>592</c:v>
+                </c:pt>
+                <c:pt idx="593">
+                  <c:v>593</c:v>
+                </c:pt>
+                <c:pt idx="594">
+                  <c:v>594</c:v>
+                </c:pt>
+                <c:pt idx="595">
+                  <c:v>595</c:v>
+                </c:pt>
+                <c:pt idx="596">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="597">
+                  <c:v>597</c:v>
+                </c:pt>
+                <c:pt idx="598">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="599">
+                  <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="600">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="601">
+                  <c:v>601</c:v>
+                </c:pt>
+                <c:pt idx="602">
+                  <c:v>602</c:v>
+                </c:pt>
+                <c:pt idx="603">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="604">
+                  <c:v>604</c:v>
+                </c:pt>
+                <c:pt idx="605">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="606">
+                  <c:v>606</c:v>
+                </c:pt>
+                <c:pt idx="607">
+                  <c:v>607</c:v>
+                </c:pt>
+                <c:pt idx="608">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="609">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="610">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="611">
+                  <c:v>611</c:v>
+                </c:pt>
+                <c:pt idx="612">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="613">
+                  <c:v>613</c:v>
+                </c:pt>
+                <c:pt idx="614">
+                  <c:v>614</c:v>
+                </c:pt>
+                <c:pt idx="615">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="616">
+                  <c:v>616</c:v>
+                </c:pt>
+                <c:pt idx="617">
+                  <c:v>617</c:v>
+                </c:pt>
+                <c:pt idx="618">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="619">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="620">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="621">
+                  <c:v>621</c:v>
+                </c:pt>
+                <c:pt idx="622">
+                  <c:v>622</c:v>
+                </c:pt>
+                <c:pt idx="623">
+                  <c:v>623</c:v>
+                </c:pt>
+                <c:pt idx="624">
+                  <c:v>624</c:v>
+                </c:pt>
+                <c:pt idx="625">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="626">
+                  <c:v>626</c:v>
+                </c:pt>
+                <c:pt idx="627">
+                  <c:v>627</c:v>
+                </c:pt>
+                <c:pt idx="628">
+                  <c:v>628</c:v>
+                </c:pt>
+                <c:pt idx="629">
+                  <c:v>629</c:v>
+                </c:pt>
+                <c:pt idx="630">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="631">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="632">
+                  <c:v>632</c:v>
+                </c:pt>
+                <c:pt idx="633">
+                  <c:v>633</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$6:$L$639</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="634"/>
+                <c:pt idx="0">
+                  <c:v>8782083.48475518</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77859064.3288778</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>171938356.896128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>266132409.362094</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>360326863.601907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>454521662.328219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>548715306.204109</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>642905962.415587</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>702788402.047124</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-250850892.164412</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-688119848.876105</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-309325079.300087</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3267009.09190203</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50416.3747997666</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7044382.40021741</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>223256286.251637</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>627645437.371032</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>790452773.025229</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>763769773.902937</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>563135206.846229</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>391695927.757651</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>266853754.019453</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>179625148.995258</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>119929169.213289</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>79675953.3050663</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>52815208.0694725</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34947611.0405758</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23038799.7715087</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15241760.0748761</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10048411.5351832</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6648697.7148517</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4428792.30388523</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2888339.62391367</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1910234.88776994</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1346919.82781456</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-290938700.063398</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-927253092.823222</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-882724806.176712</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-812836731.823738</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-742763935.323963</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-672792128.69049</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-602831968.77266</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-532761110.885392</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-462828600.867093</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-392774289.725379</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-322814350.854652</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-252811836.617243</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-182792410.045409</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-112816171.041535</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-25945626.0985502</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>32823.6248142174</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-189590672.392552</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>64165197.2165909</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>157801600.457733</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>252007579.188351</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>346207080.192696</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>440360498.845493</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>534639172.874831</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>628689036.899614</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>723102382.15295</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>806111851.452245</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>716248365.639481</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>512927330.548936</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>354587894.423353</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>240762013.716849</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>161391177.096724</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>107862303.708731</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>71502266.7748721</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>47286477.4692408</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>31424784.2376202</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>20451837.1542389</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>13797406.8674791</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8955074.3911911</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5938524.47826071</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3925257.42802046</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2621630.6050164</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1791674.45905951</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1198647.40854552</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>902094.949550716</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-461607269.867217</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-938759621.655385</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-868719629.311098</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-798887075.22649</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-728882212.068188</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-607200095.670259</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-60533148.0572319</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>329764426.517093</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>691835236.052671</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>805742750.627617</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>717846658.911202</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>514309792.751696</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>355472686.086538</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>241225095.462181</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>162056717.502847</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>108086204.782659</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>71790455.8999177</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>47461180.2940333</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>31365293.508658</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>20687678.1620315</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>13797346.066934</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>8955034.97616759</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>5997762.06350639</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>3865967.65471893</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2799538.50110377</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1732371.72279477</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1139326.89200983</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>71468.4613767355</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1258077.7247027</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1258188.06401334</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-221744782.095393</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>-905888776.889031</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>-889996257.075264</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>-819883274.346902</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>-749978617.392172</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>-679881950.556146</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>-609736118.901057</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>-540036704.859133</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>-469890264.362577</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>-399941297.800365</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>-329845639.363288</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>-259864505.235428</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>-189929568.968363</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>-119899292.148674</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>-34484432.9476187</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>854.763674618836</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>8782083.48475523</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>77859064.3288783</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>171938356.896128</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>266132409.362113</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>360326863.601887</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>454521662.328201</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>548715306.204112</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>642905962.415626</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>702788402.047125</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>-250850892.164474</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>-688119848.876057</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>-309325079.300105</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>3267009.09189374</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>50416.3748578129</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>7044382.40009309</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>223256286.251716</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>627645437.371049</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>790452773.025202</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>763769773.902925</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>563135206.84637</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>391695927.75753</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>266853754.019427</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>179625148.995231</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>119929169.213342</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>79675953.305012</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>52815208.0696089</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>34947611.0405211</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>23038799.7715087</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>15241760.0747385</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>10048411.5352382</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>6648697.71496205</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>4428792.30394046</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>2888339.623748</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>1910234.88788041</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>1346919.82764882</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>-290938700.06323</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>-927253092.82328</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>-882724806.176662</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>-812836731.823788</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>-742763935.324048</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>-672792128.690329</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>-602831968.772805</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>-532761110.885263</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>-462828600.867206</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>-392774289.725282</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>-322814350.854697</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>-252811836.617272</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>-182792410.04536</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>-112816171.041568</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>-25945626.0985356</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>32823.6248141287</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>-189590672.392525</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>64165197.2165909</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>157801600.457725</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>252007579.188371</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>346207080.192667</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>440360498.845531</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>534639172.874862</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>628689036.899562</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>723102382.152915</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>806111851.452361</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>716248365.63931</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>512927330.549028</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>354587894.423353</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>240762013.716849</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>161391177.096724</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>107862303.708839</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>71502266.7746551</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>47286477.4694591</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>31424784.2374009</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>20451837.1543487</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>13797406.8675893</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>8955074.39097054</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>5938524.47837105</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>3925257.42802046</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>2621630.6050164</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>1791674.45905951</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1198647.40854552</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>902094.949550716</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>-461607269.867217</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>-938759621.655278</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>-868719629.311205</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>-798887075.226399</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>-728882212.06861</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>-607200095.66963</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>-60533148.0575055</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>329764426.516959</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>691835236.052938</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>805742750.627475</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>717846658.911113</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>514309792.751788</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>355472686.086639</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>241225095.461974</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>162056717.502846</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>108086204.78255</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>71790455.9004604</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>47461180.2935969</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>31365293.508987</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>20687678.1613716</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>13797346.0675948</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>8955034.97594711</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>5997762.06350639</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>3865967.65471893</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>2799538.50132471</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>1732371.72235284</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>1139326.89223082</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>71468.4613767355</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>1258077.7247027</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>1258188.06401334</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>-221744782.095172</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>-905888776.889698</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>-889996257.074625</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>-819883274.346918</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>-749978617.392358</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>-679881950.556146</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>-609736118.901334</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>-540036704.858856</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>-469890264.362577</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>-399941297.800274</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>-329845639.363379</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>-259864505.235487</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>-189929568.968304</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>-119899292.148674</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>-34484432.9476073</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>854.76367391579</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>8782083.48475523</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>77859064.3288783</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>171938356.896128</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>266132409.362113</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>360326863.601887</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>454521662.328201</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>548715306.204112</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>642905962.415626</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>702788402.047125</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>-250850892.164474</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>-688119848.876057</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>-309325079.300105</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>3267009.09189374</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>50416.3748578129</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>7044382.40009309</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>223256286.251716</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>627645437.371049</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>790452773.025357</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>763769773.902594</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>563135206.846549</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>391695927.75753</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>266853754.01922</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>179625148.995652</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>119929169.213129</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>79675953.305012</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>52815208.0696089</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>34947611.0403018</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>23038799.7717283</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>15241760.0749588</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>10048411.5352384</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>6648697.71474141</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>4428792.30371961</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>2888339.62374796</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>1910234.88810135</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>1346919.82809081</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>-290938700.064124</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>-927253092.822816</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>-882724806.176461</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>-812836731.823989</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>-742763935.323879</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>-672792128.690804</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>-602831968.772225</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>-532761110.885779</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>-462828600.866753</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>-392774289.725671</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>-322814350.854518</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>-252811836.617157</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>-182792410.045558</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>-112816171.041434</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>-25945626.0985842</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>32823.6248143062</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>-189590672.392492</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>64165197.2165834</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>157801600.457769</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>252007579.18829</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>346207080.192784</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>440360498.845377</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>534639172.874949</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>628689036.899439</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>723102382.153038</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>806111851.452361</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>716248365.639488</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>512927330.548651</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>354587894.423549</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>240762013.717058</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>161391177.096513</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>107862303.708623</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>71502266.7748715</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>47286477.4694591</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>31424784.2374009</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>20451837.1545688</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>13797406.8671487</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>8955074.39141165</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>5938524.47815037</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>3925257.42779959</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>2621630.60523729</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>1791674.45928048</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>1198647.40832453</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>902094.949550716</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>-461607269.867438</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>-938759621.655049</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>-868719629.311205</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>-798887075.226399</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>-728882212.068279</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>-607200095.670259</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>-60533148.0572319</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>329764426.516959</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>691835236.052938</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>805742750.627475</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>717846658.911113</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>514309792.751788</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>355472686.086639</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>241225095.461974</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>162056717.502846</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>108086204.782982</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>71790455.8995925</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>47461180.2940329</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>31365293.508987</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>20687678.1618117</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>13797346.0671544</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>8955034.97594711</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>5997762.06306484</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>3865967.65560228</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>2799538.50044106</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>1732371.7232367</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>1139326.89178885</c:v>
+                </c:pt>
+                <c:pt idx="451">
+                  <c:v>71468.4613767355</c:v>
+                </c:pt>
+                <c:pt idx="452">
+                  <c:v>1258077.72426066</c:v>
+                </c:pt>
+                <c:pt idx="453">
+                  <c:v>1258188.06445538</c:v>
+                </c:pt>
+                <c:pt idx="454">
+                  <c:v>-221744782.095172</c:v>
+                </c:pt>
+                <c:pt idx="455">
+                  <c:v>-905888776.889263</c:v>
+                </c:pt>
+                <c:pt idx="456">
+                  <c:v>-889996257.075061</c:v>
+                </c:pt>
+                <c:pt idx="457">
+                  <c:v>-819883274.347291</c:v>
+                </c:pt>
+                <c:pt idx="458">
+                  <c:v>-749978617.391986</c:v>
+                </c:pt>
+                <c:pt idx="459">
+                  <c:v>-679881950.556146</c:v>
+                </c:pt>
+                <c:pt idx="460">
+                  <c:v>-609736118.901057</c:v>
+                </c:pt>
+                <c:pt idx="461">
+                  <c:v>-540036704.859133</c:v>
+                </c:pt>
+                <c:pt idx="462">
+                  <c:v>-469890264.362577</c:v>
+                </c:pt>
+                <c:pt idx="463">
+                  <c:v>-399941297.800456</c:v>
+                </c:pt>
+                <c:pt idx="464">
+                  <c:v>-329845639.363197</c:v>
+                </c:pt>
+                <c:pt idx="465">
+                  <c:v>-259864505.235368</c:v>
+                </c:pt>
+                <c:pt idx="466">
+                  <c:v>-189929568.968422</c:v>
+                </c:pt>
+                <c:pt idx="467">
+                  <c:v>-119899292.148674</c:v>
+                </c:pt>
+                <c:pt idx="468">
+                  <c:v>-34484432.9476073</c:v>
+                </c:pt>
+                <c:pt idx="469">
+                  <c:v>854.76367391579</c:v>
+                </c:pt>
+                <c:pt idx="470">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="471">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="472">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="473">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="474">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="475">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="476">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="477">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="478">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="479">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="480">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="481">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="482">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="483">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="484">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="485">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="486">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="487">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="488">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="489">
+                  <c:v>8782083.48475523</c:v>
+                </c:pt>
+                <c:pt idx="490">
+                  <c:v>77859064.3288783</c:v>
+                </c:pt>
+                <c:pt idx="491">
+                  <c:v>171938356.896128</c:v>
+                </c:pt>
+                <c:pt idx="492">
+                  <c:v>266132409.362113</c:v>
+                </c:pt>
+                <c:pt idx="493">
+                  <c:v>360326863.601887</c:v>
+                </c:pt>
+                <c:pt idx="494">
+                  <c:v>454521662.328201</c:v>
+                </c:pt>
+                <c:pt idx="495">
+                  <c:v>548715306.204112</c:v>
+                </c:pt>
+                <c:pt idx="496">
+                  <c:v>642905962.415626</c:v>
+                </c:pt>
+                <c:pt idx="497">
+                  <c:v>702788402.047125</c:v>
+                </c:pt>
+                <c:pt idx="498">
+                  <c:v>-250850892.164474</c:v>
+                </c:pt>
+                <c:pt idx="499">
+                  <c:v>-688119848.876057</c:v>
+                </c:pt>
+                <c:pt idx="500">
+                  <c:v>-309325079.300105</c:v>
+                </c:pt>
+                <c:pt idx="501">
+                  <c:v>3267009.09189374</c:v>
+                </c:pt>
+                <c:pt idx="502">
+                  <c:v>50416.3748578129</c:v>
+                </c:pt>
+                <c:pt idx="503">
+                  <c:v>7044382.40009309</c:v>
+                </c:pt>
+                <c:pt idx="504">
+                  <c:v>223256286.251716</c:v>
+                </c:pt>
+                <c:pt idx="505">
+                  <c:v>627645437.370772</c:v>
+                </c:pt>
+                <c:pt idx="506">
+                  <c:v>790452773.025631</c:v>
+                </c:pt>
+                <c:pt idx="507">
+                  <c:v>763769773.902941</c:v>
+                </c:pt>
+                <c:pt idx="508">
+                  <c:v>563135206.845812</c:v>
+                </c:pt>
+                <c:pt idx="509">
+                  <c:v>391695927.757917</c:v>
+                </c:pt>
+                <c:pt idx="510">
+                  <c:v>266853754.019635</c:v>
+                </c:pt>
+                <c:pt idx="511">
+                  <c:v>179625148.99481</c:v>
+                </c:pt>
+                <c:pt idx="512">
+                  <c:v>119929169.213555</c:v>
+                </c:pt>
+                <c:pt idx="513">
+                  <c:v>79675953.3054463</c:v>
+                </c:pt>
+                <c:pt idx="514">
+                  <c:v>52815208.0691736</c:v>
+                </c:pt>
+                <c:pt idx="515">
+                  <c:v>34947611.0403018</c:v>
+                </c:pt>
+                <c:pt idx="516">
+                  <c:v>23038799.7717283</c:v>
+                </c:pt>
+                <c:pt idx="517">
+                  <c:v>15241760.0745181</c:v>
+                </c:pt>
+                <c:pt idx="518">
+                  <c:v>10048411.5356792</c:v>
+                </c:pt>
+                <c:pt idx="519">
+                  <c:v>6648697.71474141</c:v>
+                </c:pt>
+                <c:pt idx="520">
+                  <c:v>4428792.30371961</c:v>
+                </c:pt>
+                <c:pt idx="521">
+                  <c:v>2888339.6241898</c:v>
+                </c:pt>
+                <c:pt idx="522">
+                  <c:v>1910234.88765948</c:v>
+                </c:pt>
+                <c:pt idx="523">
+                  <c:v>1346919.82764882</c:v>
+                </c:pt>
+                <c:pt idx="524">
+                  <c:v>-290938700.062788</c:v>
+                </c:pt>
+                <c:pt idx="525">
+                  <c:v>-927253092.823743</c:v>
+                </c:pt>
+                <c:pt idx="526">
+                  <c:v>-882724806.177264</c:v>
+                </c:pt>
+                <c:pt idx="527">
+                  <c:v>-812836731.823186</c:v>
+                </c:pt>
+                <c:pt idx="528">
+                  <c:v>-742763935.323879</c:v>
+                </c:pt>
+                <c:pt idx="529">
+                  <c:v>-672792128.690498</c:v>
+                </c:pt>
+                <c:pt idx="530">
+                  <c:v>-602831968.772805</c:v>
+                </c:pt>
+                <c:pt idx="531">
+                  <c:v>-532761110.885263</c:v>
+                </c:pt>
+                <c:pt idx="532">
+                  <c:v>-462828600.867206</c:v>
+                </c:pt>
+                <c:pt idx="533">
+                  <c:v>-392774289.725282</c:v>
+                </c:pt>
+                <c:pt idx="534">
+                  <c:v>-322814350.854697</c:v>
+                </c:pt>
+                <c:pt idx="535">
+                  <c:v>-252811836.617272</c:v>
+                </c:pt>
+                <c:pt idx="536">
+                  <c:v>-182792410.04536</c:v>
+                </c:pt>
+                <c:pt idx="537">
+                  <c:v>-112816171.041568</c:v>
+                </c:pt>
+                <c:pt idx="538">
+                  <c:v>-25945626.0985454</c:v>
+                </c:pt>
+                <c:pt idx="539">
+                  <c:v>32823.6248143062</c:v>
+                </c:pt>
+                <c:pt idx="540">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="541">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="542">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="543">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="544">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="545">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="546">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="547">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="548">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="549">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="550">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="551">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="552">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="553">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="554">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="555">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="556">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="557">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="558">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="559">
+                  <c:v>-189590672.392492</c:v>
+                </c:pt>
+                <c:pt idx="560">
+                  <c:v>64165197.2165834</c:v>
+                </c:pt>
+                <c:pt idx="561">
+                  <c:v>157801600.457831</c:v>
+                </c:pt>
+                <c:pt idx="562">
+                  <c:v>252007579.18813</c:v>
+                </c:pt>
+                <c:pt idx="563">
+                  <c:v>346207080.193019</c:v>
+                </c:pt>
+                <c:pt idx="564">
+                  <c:v>440360498.845241</c:v>
+                </c:pt>
+                <c:pt idx="565">
+                  <c:v>534639172.874739</c:v>
+                </c:pt>
+                <c:pt idx="566">
+                  <c:v>628689036.899895</c:v>
+                </c:pt>
+                <c:pt idx="567">
+                  <c:v>723102382.153075</c:v>
+                </c:pt>
+                <c:pt idx="568">
+                  <c:v>806111851.451756</c:v>
+                </c:pt>
+                <c:pt idx="569">
+                  <c:v>716248365.639459</c:v>
+                </c:pt>
+                <c:pt idx="570">
+                  <c:v>512927330.54979</c:v>
+                </c:pt>
+                <c:pt idx="571">
+                  <c:v>354587894.422764</c:v>
+                </c:pt>
+                <c:pt idx="572">
+                  <c:v>240762013.716223</c:v>
+                </c:pt>
+                <c:pt idx="573">
+                  <c:v>161391177.097781</c:v>
+                </c:pt>
+                <c:pt idx="574">
+                  <c:v>107862303.708195</c:v>
+                </c:pt>
+                <c:pt idx="575">
+                  <c:v>71502266.7753067</c:v>
+                </c:pt>
+                <c:pt idx="576">
+                  <c:v>47286477.4685856</c:v>
+                </c:pt>
+                <c:pt idx="577">
+                  <c:v>31424784.238278</c:v>
+                </c:pt>
+                <c:pt idx="578">
+                  <c:v>20451837.1536892</c:v>
+                </c:pt>
+                <c:pt idx="579">
+                  <c:v>13797406.867589</c:v>
+                </c:pt>
+                <c:pt idx="580">
+                  <c:v>8955074.39141165</c:v>
+                </c:pt>
+                <c:pt idx="581">
+                  <c:v>5938524.47815037</c:v>
+                </c:pt>
+                <c:pt idx="582">
+                  <c:v>3925257.42824133</c:v>
+                </c:pt>
+                <c:pt idx="583">
+                  <c:v>2621630.60479551</c:v>
+                </c:pt>
+                <c:pt idx="584">
+                  <c:v>1791674.45839658</c:v>
+                </c:pt>
+                <c:pt idx="585">
+                  <c:v>1198647.40920847</c:v>
+                </c:pt>
+                <c:pt idx="586">
+                  <c:v>902094.949992762</c:v>
+                </c:pt>
+                <c:pt idx="587">
+                  <c:v>-461607269.867453</c:v>
+                </c:pt>
+                <c:pt idx="588">
+                  <c:v>-938759621.655935</c:v>
+                </c:pt>
+                <c:pt idx="589">
+                  <c:v>-868719629.310778</c:v>
+                </c:pt>
+                <c:pt idx="590">
+                  <c:v>-798887075.226036</c:v>
+                </c:pt>
+                <c:pt idx="591">
+                  <c:v>-728882212.068973</c:v>
+                </c:pt>
+                <c:pt idx="592">
+                  <c:v>-607200095.66963</c:v>
+                </c:pt>
+                <c:pt idx="593">
+                  <c:v>-60533148.0575055</c:v>
+                </c:pt>
+                <c:pt idx="594">
+                  <c:v>329764426.516959</c:v>
+                </c:pt>
+                <c:pt idx="595">
+                  <c:v>691835236.052938</c:v>
+                </c:pt>
+                <c:pt idx="596">
+                  <c:v>805742750.627475</c:v>
+                </c:pt>
+                <c:pt idx="597">
+                  <c:v>717846658.910757</c:v>
+                </c:pt>
+                <c:pt idx="598">
+                  <c:v>514309792.752154</c:v>
+                </c:pt>
+                <c:pt idx="599">
+                  <c:v>355472686.087044</c:v>
+                </c:pt>
+                <c:pt idx="600">
+                  <c:v>241225095.461147</c:v>
+                </c:pt>
+                <c:pt idx="601">
+                  <c:v>162056717.503692</c:v>
+                </c:pt>
+                <c:pt idx="602">
+                  <c:v>108086204.782122</c:v>
+                </c:pt>
+                <c:pt idx="603">
+                  <c:v>71790455.9000252</c:v>
+                </c:pt>
+                <c:pt idx="604">
+                  <c:v>47461180.2944704</c:v>
+                </c:pt>
+                <c:pt idx="605">
+                  <c:v>31365293.508549</c:v>
+                </c:pt>
+                <c:pt idx="606">
+                  <c:v>20687678.1613716</c:v>
+                </c:pt>
+                <c:pt idx="607">
+                  <c:v>13797346.067154</c:v>
+                </c:pt>
+                <c:pt idx="608">
+                  <c:v>8955034.97638807</c:v>
+                </c:pt>
+                <c:pt idx="609">
+                  <c:v>5997762.06394794</c:v>
+                </c:pt>
+                <c:pt idx="610">
+                  <c:v>3865967.65383556</c:v>
+                </c:pt>
+                <c:pt idx="611">
+                  <c:v>2799538.50132462</c:v>
+                </c:pt>
+                <c:pt idx="612">
+                  <c:v>1732371.7232367</c:v>
+                </c:pt>
+                <c:pt idx="613">
+                  <c:v>1139326.89178885</c:v>
+                </c:pt>
+                <c:pt idx="614">
+                  <c:v>71468.4613767355</c:v>
+                </c:pt>
+                <c:pt idx="615">
+                  <c:v>1258077.72514475</c:v>
+                </c:pt>
+                <c:pt idx="616">
+                  <c:v>1258188.06357129</c:v>
+                </c:pt>
+                <c:pt idx="617">
+                  <c:v>-221744782.096056</c:v>
+                </c:pt>
+                <c:pt idx="618">
+                  <c:v>-905888776.887898</c:v>
+                </c:pt>
+                <c:pt idx="619">
+                  <c:v>-889996257.075903</c:v>
+                </c:pt>
+                <c:pt idx="620">
+                  <c:v>-819883274.346886</c:v>
+                </c:pt>
+                <c:pt idx="621">
+                  <c:v>-749978617.391986</c:v>
+                </c:pt>
+                <c:pt idx="622">
+                  <c:v>-679881950.556146</c:v>
+                </c:pt>
+                <c:pt idx="623">
+                  <c:v>-609736118.900779</c:v>
+                </c:pt>
+                <c:pt idx="624">
+                  <c:v>-540036704.85941</c:v>
+                </c:pt>
+                <c:pt idx="625">
+                  <c:v>-469890264.362577</c:v>
+                </c:pt>
+                <c:pt idx="626">
+                  <c:v>-399941297.800274</c:v>
+                </c:pt>
+                <c:pt idx="627">
+                  <c:v>-329845639.363379</c:v>
+                </c:pt>
+                <c:pt idx="628">
+                  <c:v>-259864505.235487</c:v>
+                </c:pt>
+                <c:pt idx="629">
+                  <c:v>-189929568.968304</c:v>
+                </c:pt>
+                <c:pt idx="630">
+                  <c:v>-119899292.148674</c:v>
+                </c:pt>
+                <c:pt idx="631">
+                  <c:v>-34484432.94763</c:v>
+                </c:pt>
+                <c:pt idx="632">
+                  <c:v>35027.149597897</c:v>
+                </c:pt>
+                <c:pt idx="633">
+                  <c:v>35027.149597897</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="17497548"/>
+        <c:axId val="23684352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="17497548"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Temps [s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="##0.0E+0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="23684352"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="23684352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Puissance [W]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="##0.0E+0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17497548"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>522720</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>106200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>907560</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>212400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1963080" y="946440"/>
+        <a:ext cx="11906280" cy="6827040"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -338,7 +4552,7 @@
   <dimension ref="A1:O639"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.43359375" defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30841,7 +35055,7 @@
       </c>
       <c r="D638" s="1" t="n">
         <f aca="false">C639-C638</f>
-        <v>4985.75183105468</v>
+        <v>0</v>
       </c>
       <c r="E638" s="1" t="n">
         <f aca="false">($B$2+$C$2*$A$2)+($D$2+$E$2*$A$2)*C638+($F$2+$G$2*$A$2)*C638^2</f>
@@ -30849,7 +35063,7 @@
       </c>
       <c r="F638" s="1" t="n">
         <f aca="false">$A$2*D638+$A$2*$I$2*SIN($H$2)+E638</f>
-        <v>349002629402.609</v>
+        <v>1228.7818011024</v>
       </c>
       <c r="G638" s="1" t="n">
         <f aca="false">$L$2*B638</f>
@@ -30873,7 +35087,7 @@
       </c>
       <c r="L638" s="1" t="n">
         <f aca="false">$O$2+F638*C638</f>
-        <v>7711152665.29193</v>
+        <v>35027.149597897</v>
       </c>
     </row>
     <row r="639" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30884,20 +35098,20 @@
         <v>4985.77392578124</v>
       </c>
       <c r="C639" s="1" t="n">
-        <f aca="false">B639-B640</f>
-        <v>4985.77392578124</v>
+        <f aca="false">C638</f>
+        <v>0.0220947265597715</v>
       </c>
       <c r="D639" s="1" t="n">
-        <f aca="false">C639-C640</f>
-        <v>4985.77392578124</v>
+        <f aca="false">D638</f>
+        <v>0</v>
       </c>
       <c r="E639" s="1" t="n">
         <f aca="false">($B$2+$C$2*$A$2)+($D$2+$E$2*$A$2)*C639+($F$2+$G$2*$A$2)*C639^2</f>
-        <v>117249678.955401</v>
+        <v>1228.7818011024</v>
       </c>
       <c r="F639" s="1" t="n">
         <f aca="false">$A$2*D639+$A$2*$I$2*SIN($H$2)+E639</f>
-        <v>349121424483.642</v>
+        <v>1228.7818011024</v>
       </c>
       <c r="G639" s="1" t="n">
         <f aca="false">$L$2*B639</f>
@@ -30921,7 +35135,7 @@
       </c>
       <c r="L639" s="1" t="n">
         <f aca="false">$O$2+F639*C639</f>
-        <v>1740640495157150</v>
+        <v>35027.149597897</v>
       </c>
     </row>
   </sheetData>
@@ -30932,5 +35146,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>